<commit_message>
Trying to fix the pdf writer
</commit_message>
<xml_diff>
--- a/registrations_April_24.xlsx
+++ b/registrations_April_24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\Documents\Repos\ABLE_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61E32A39-15E1-41BC-BDE2-1939DF031365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F88EEFD-F1BF-4DED-B725-5325C52759A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18255" yWindow="390" windowWidth="19095" windowHeight="19770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registrations" sheetId="6" r:id="rId1"/>
@@ -4028,34 +4028,34 @@
     <t>Presenter Person11</t>
   </si>
   <si>
-    <t>TR1</t>
-  </si>
-  <si>
-    <t>TR2</t>
-  </si>
-  <si>
-    <t>TR3</t>
-  </si>
-  <si>
-    <t>TR4</t>
-  </si>
-  <si>
-    <t>TR5</t>
-  </si>
-  <si>
-    <t>TR6</t>
-  </si>
-  <si>
-    <t>TR7</t>
-  </si>
-  <si>
-    <t>TR8</t>
-  </si>
-  <si>
-    <t>TR9</t>
-  </si>
-  <si>
-    <t>TR10</t>
+    <t>TR12</t>
+  </si>
+  <si>
+    <t>TR13</t>
+  </si>
+  <si>
+    <t>TR14</t>
+  </si>
+  <si>
+    <t>TR15</t>
+  </si>
+  <si>
+    <t>TR16</t>
+  </si>
+  <si>
+    <t>TR17</t>
+  </si>
+  <si>
+    <t>TR18</t>
+  </si>
+  <si>
+    <t>TR19</t>
+  </si>
+  <si>
+    <t>TR20</t>
+  </si>
+  <si>
+    <t>TR21</t>
   </si>
 </sst>
 </file>
@@ -4913,8 +4913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{661C42CE-B24A-44A3-9567-541D64117560}">
   <dimension ref="A1:AV136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AD11" sqref="AD11"/>
+    <sheetView topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AC28" sqref="AC28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20132,7 +20132,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20191,7 +20191,7 @@
         <v>611</v>
       </c>
       <c r="C4" t="s">
-        <v>1299</v>
+        <v>1307</v>
       </c>
       <c r="D4" t="s">
         <v>1311</v>
@@ -20205,7 +20205,7 @@
         <v>613</v>
       </c>
       <c r="C5" t="s">
-        <v>1300</v>
+        <v>1308</v>
       </c>
       <c r="D5" t="s">
         <v>1312</v>
@@ -20219,7 +20219,7 @@
         <v>604</v>
       </c>
       <c r="C6" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="D6" t="s">
         <v>1313</v>
@@ -20233,7 +20233,7 @@
         <v>605</v>
       </c>
       <c r="C7" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="D7" t="s">
         <v>1314</v>
@@ -20247,7 +20247,7 @@
         <v>606</v>
       </c>
       <c r="C8" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="D8" t="s">
         <v>1315</v>
@@ -20261,7 +20261,7 @@
         <v>607</v>
       </c>
       <c r="C9" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="D9" t="s">
         <v>1316</v>
@@ -20275,7 +20275,7 @@
         <v>608</v>
       </c>
       <c r="C10" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="D10" t="s">
         <v>1317</v>
@@ -20289,7 +20289,7 @@
         <v>612</v>
       </c>
       <c r="C11" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="D11" t="s">
         <v>1318</v>
@@ -20303,7 +20303,7 @@
         <v>609</v>
       </c>
       <c r="C12" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="D12" t="s">
         <v>1319</v>
@@ -20317,7 +20317,7 @@
         <v>610</v>
       </c>
       <c r="C13" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="D13" t="s">
         <v>1320</v>
@@ -20337,8 +20337,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Final updates to error handling
</commit_message>
<xml_diff>
--- a/registrations_April_24.xlsx
+++ b/registrations_April_24.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zacha\Documents\Repos\ABLE_App\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F88EEFD-F1BF-4DED-B725-5325C52759A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4B41CA-B17B-49CA-B95B-2BFAB258AD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registrations" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3700" uniqueCount="1331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3700" uniqueCount="1332">
   <si>
     <t>first_name</t>
   </si>
@@ -3956,9 +3956,6 @@
     <t>802-304-8071</t>
   </si>
   <si>
-    <t>Room location</t>
-  </si>
-  <si>
     <t>WR1</t>
   </si>
   <si>
@@ -4056,6 +4053,12 @@
   </si>
   <si>
     <t>TR21</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>location</t>
   </si>
 </sst>
 </file>
@@ -20131,8 +20134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20149,10 +20152,10 @@
         <v>602</v>
       </c>
       <c r="C1" t="s">
-        <v>1297</v>
+        <v>1331</v>
       </c>
       <c r="D1" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -20177,10 +20180,10 @@
         <v>603</v>
       </c>
       <c r="C3" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="D3" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -20191,10 +20194,10 @@
         <v>611</v>
       </c>
       <c r="C4" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="D4" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -20205,10 +20208,10 @@
         <v>613</v>
       </c>
       <c r="C5" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="D5" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -20219,10 +20222,10 @@
         <v>604</v>
       </c>
       <c r="C6" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="D6" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -20233,10 +20236,10 @@
         <v>605</v>
       </c>
       <c r="C7" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="D7" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -20247,10 +20250,10 @@
         <v>606</v>
       </c>
       <c r="C8" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="D8" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -20261,10 +20264,10 @@
         <v>607</v>
       </c>
       <c r="C9" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="D9" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -20275,10 +20278,10 @@
         <v>608</v>
       </c>
       <c r="C10" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="D10" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -20289,10 +20292,10 @@
         <v>612</v>
       </c>
       <c r="C11" t="s">
-        <v>1304</v>
+        <v>1303</v>
       </c>
       <c r="D11" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -20303,10 +20306,10 @@
         <v>609</v>
       </c>
       <c r="C12" t="s">
-        <v>1305</v>
+        <v>1304</v>
       </c>
       <c r="D12" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -20317,10 +20320,10 @@
         <v>610</v>
       </c>
       <c r="C13" t="s">
-        <v>1306</v>
+        <v>1305</v>
       </c>
       <c r="D13" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
     </row>
   </sheetData>
@@ -20337,8 +20340,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20351,10 +20354,10 @@
         <v>602</v>
       </c>
       <c r="C1" t="s">
-        <v>1297</v>
+        <v>1330</v>
       </c>
       <c r="D1" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -20379,10 +20382,10 @@
         <v>614</v>
       </c>
       <c r="C3" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="D3" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -20393,10 +20396,10 @@
         <v>615</v>
       </c>
       <c r="C4" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="D4" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -20407,10 +20410,10 @@
         <v>616</v>
       </c>
       <c r="C5" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="D5" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -20421,10 +20424,10 @@
         <v>617</v>
       </c>
       <c r="C6" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="D6" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -20435,10 +20438,10 @@
         <v>618</v>
       </c>
       <c r="C7" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="D7" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -20449,10 +20452,10 @@
         <v>619</v>
       </c>
       <c r="C8" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="D8" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -20463,10 +20466,10 @@
         <v>620</v>
       </c>
       <c r="C9" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="D9" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -20477,10 +20480,10 @@
         <v>622</v>
       </c>
       <c r="C10" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="D10" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -20491,10 +20494,10 @@
         <v>621</v>
       </c>
       <c r="C11" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="D11" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -20505,10 +20508,10 @@
         <v>623</v>
       </c>
       <c r="C12" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="D12" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
     </row>
   </sheetData>

</xml_diff>